<commit_message>
New asset upload is running
</commit_message>
<xml_diff>
--- a/public/new assets.xlsx
+++ b/public/new assets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ams\next-asset-management-system\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0B82C7-905F-480A-924A-B9DACF571436}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A93DD04-A548-48B1-94FC-D98FB165ED05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="27">
   <si>
     <t>UPS</t>
   </si>
@@ -1094,13 +1094,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F15954-12F9-4AC8-97D5-364525F0D95D}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -2562,6 +2565,26 @@
         <v>29807.72</v>
       </c>
     </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>150000026580</v>
+      </c>
+      <c r="B74" s="5">
+        <v>45767</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" s="7">
+        <v>31032</v>
+      </c>
+      <c r="E74" s="7">
+        <v>-1224.28</v>
+      </c>
+      <c r="F74" s="12">
+        <v>29807.72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>